<commit_message>
Changed short name in profile spreadsheets for Simplifier update
</commit_message>
<xml_diff>
--- a/output/access-diagnosticreport-gen-pat.xlsx
+++ b/output/access-diagnosticreport-gen-pat.xlsx
@@ -168,7 +168,7 @@
     <t/>
   </si>
   <si>
-    <t>A Diagnostic report - a combination of request information, atomic results, images, interpretation, as well as formatted reports</t>
+    <t>DiagnosticReport General Lab (Patient) Profile</t>
   </si>
   <si>
     <t>Expected requirements for the DiagnosticReport resource when reflecting general lab result data based on existing source mappings.</t>
@@ -1235,7 +1235,7 @@
     <col min="8" max="8" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="114.69140625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="65.7890625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>